<commit_message>
updated background to white, centered eyes on face stimuli, added audio cues for sync
</commit_message>
<xml_diff>
--- a/Emotion/stimuli.xlsx
+++ b/Emotion/stimuli.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/llevinson/Google Drive UW/SCH_Anxiety_Tasks/Emotion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/llevinson/Documents/SCH_Anxiety_Tasks/Emotion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5B9EE4-25ED-794D-8DAF-AF9152CA855A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F907E011-6B97-B64F-8277-F297D8F46865}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="16860" windowHeight="17040" xr2:uid="{1E8879B0-F6DF-7948-B23A-C8B6A5004E47}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21580" windowHeight="17040" xr2:uid="{1E8879B0-F6DF-7948-B23A-C8B6A5004E47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,51 +39,6 @@
     <t>ImageFile</t>
   </si>
   <si>
-    <t>Images/07F_AN_O.jpg</t>
-  </si>
-  <si>
-    <t>Images/07F_FE_O.jpg</t>
-  </si>
-  <si>
-    <t>Images/07F_HA_O.jpg</t>
-  </si>
-  <si>
-    <t>Images/07F_NE_O.jpg</t>
-  </si>
-  <si>
-    <t>Images/13F_AN_O_new.jpg</t>
-  </si>
-  <si>
-    <t>Images/13F_FE_O.jpg</t>
-  </si>
-  <si>
-    <t>Images/13F_HA_O.jpg</t>
-  </si>
-  <si>
-    <t>Images/13F_NE_O.jpg</t>
-  </si>
-  <si>
-    <t>Images/18F_AN_O.jpg</t>
-  </si>
-  <si>
-    <t>Images/18F_FE_O.jpg</t>
-  </si>
-  <si>
-    <t>Images/18F_HA_O.jpg</t>
-  </si>
-  <si>
-    <t>Images/18F_NE_O.jpg</t>
-  </si>
-  <si>
-    <t>Images/House1.jpg</t>
-  </si>
-  <si>
-    <t>Images/House2.jpg</t>
-  </si>
-  <si>
-    <t>Images/House3.jpg</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -103,6 +58,51 @@
   </si>
   <si>
     <t>Num</t>
+  </si>
+  <si>
+    <t>Images/07F_AN_O.png</t>
+  </si>
+  <si>
+    <t>Images/07F_FE_O.png</t>
+  </si>
+  <si>
+    <t>Images/07F_HA_O.png</t>
+  </si>
+  <si>
+    <t>Images/07F_NE_O.png</t>
+  </si>
+  <si>
+    <t>Images/13F_AN_O_new.png</t>
+  </si>
+  <si>
+    <t>Images/13F_FE_O.png</t>
+  </si>
+  <si>
+    <t>Images/13F_HA_O.png</t>
+  </si>
+  <si>
+    <t>Images/13F_NE_O.png</t>
+  </si>
+  <si>
+    <t>Images/18F_AN_O.png</t>
+  </si>
+  <si>
+    <t>Images/18F_FE_O.png</t>
+  </si>
+  <si>
+    <t>Images/18F_HA_O.png</t>
+  </si>
+  <si>
+    <t>Images/18F_NE_O.png</t>
+  </si>
+  <si>
+    <t>Images/House1.png</t>
+  </si>
+  <si>
+    <t>Images/House2.png</t>
+  </si>
+  <si>
+    <t>Images/House3.png</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -470,18 +470,18 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -489,10 +489,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -500,10 +500,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -511,10 +511,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -522,10 +522,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -533,10 +533,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -544,10 +544,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C8">
         <v>6</v>
@@ -555,10 +555,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>7</v>
@@ -566,10 +566,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>8</v>
@@ -577,10 +577,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>9</v>
@@ -588,10 +588,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C12">
         <v>10</v>
@@ -599,10 +599,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C13">
         <v>11</v>
@@ -610,10 +610,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C14">
         <v>12</v>
@@ -621,10 +621,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C15">
         <v>13</v>
@@ -632,10 +632,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C16">
         <v>14</v>

</xml_diff>